<commit_message>
excel and use case edit 1
</commit_message>
<xml_diff>
--- a/Documents/Database.xlsx
+++ b/Documents/Database.xlsx
@@ -5,22 +5,23 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Group15\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Group15 Git\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8485B7E5-F03C-42F7-A702-A04F40A674A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAB19340-05EF-4912-8D55-938A1EA5E6C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Database" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="67">
   <si>
     <t>Farmer</t>
   </si>
@@ -92,12 +93,6 @@
   </si>
   <si>
     <t>Primary Key (Auto Generated) int</t>
-  </si>
-  <si>
-    <t>Foreign key(Customer)</t>
-  </si>
-  <si>
-    <t>Foreign key(Property)</t>
   </si>
   <si>
     <t>double</t>
@@ -193,9 +188,6 @@
     <t>Foregin key(address)</t>
   </si>
   <si>
-    <t>Foreign key()</t>
-  </si>
-  <si>
     <t>equipment_image</t>
   </si>
   <si>
@@ -203,9 +195,6 @@
   </si>
   <si>
     <t>text</t>
-  </si>
-  <si>
-    <t>Foreign key(renter)</t>
   </si>
   <si>
     <t>Feedback</t>
@@ -240,12 +229,21 @@
   <si>
     <t>Foreign key(farmer/renter)</t>
   </si>
+  <si>
+    <t>Foreign key(Farmer)</t>
+  </si>
+  <si>
+    <t>Foreign key(Renter)</t>
+  </si>
+  <si>
+    <t>Foreign key(Equipment)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -354,6 +352,19 @@
       <sz val="10"/>
       <color rgb="FF4285F4"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="4"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="10">
@@ -485,7 +496,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -541,9 +552,18 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -559,14 +579,9 @@
     <xf numFmtId="0" fontId="11" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -788,8 +803,8 @@
   </sheetPr>
   <dimension ref="A1:AA995"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I42" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -899,7 +914,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -962,7 +977,7 @@
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="10" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>4</v>
@@ -1081,16 +1096,16 @@
     <row r="10" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
-      <c r="C10" s="41" t="s">
+      <c r="C10" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="D10" s="37"/>
-      <c r="E10" s="37"/>
-      <c r="F10" s="37"/>
-      <c r="G10" s="37"/>
-      <c r="H10" s="37"/>
-      <c r="I10" s="37"/>
-      <c r="J10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="38"/>
+      <c r="J10" s="39"/>
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
       <c r="M10" s="4"/>
@@ -1122,7 +1137,7 @@
         <v>7</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G11" s="14" t="s">
         <v>8</v>
@@ -1131,10 +1146,10 @@
         <v>9</v>
       </c>
       <c r="I11" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
-      <c r="J11" s="16" t="s">
-        <v>46</v>
+      <c r="J11" s="48" t="s">
+        <v>44</v>
       </c>
       <c r="L11" s="4"/>
       <c r="M11" s="4"/>
@@ -1161,23 +1176,23 @@
       <c r="D12" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="E12" s="27" t="s">
         <v>12</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G12" s="8" t="s">
         <v>12</v>
       </c>
       <c r="H12" s="14" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I12" s="14" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="J12" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
@@ -1284,17 +1299,17 @@
     <row r="16" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
-      <c r="C16" s="40" t="s">
+      <c r="C16" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="37"/>
-      <c r="E16" s="37"/>
-      <c r="F16" s="37"/>
-      <c r="G16" s="37"/>
-      <c r="H16" s="37"/>
-      <c r="I16" s="37"/>
-      <c r="J16" s="37"/>
-      <c r="K16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="38"/>
+      <c r="J16" s="38"/>
+      <c r="K16" s="39"/>
       <c r="L16" s="4"/>
       <c r="M16" s="4"/>
       <c r="N16" s="4"/>
@@ -1322,10 +1337,10 @@
         <v>15</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G17" s="14" t="s">
         <v>16</v>
@@ -1337,10 +1352,10 @@
         <v>10</v>
       </c>
       <c r="J17" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="K17" s="16" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="M17" s="4"/>
       <c r="N17" s="4"/>
@@ -1382,10 +1397,10 @@
         <v>12</v>
       </c>
       <c r="J18" s="14" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="K18" s="8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="M18" s="4"/>
       <c r="N18" s="4"/>
@@ -1491,13 +1506,13 @@
     </row>
     <row r="22" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B22" s="2"/>
-      <c r="C22" s="43" t="s">
+      <c r="C22" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="D22" s="37"/>
-      <c r="E22" s="37"/>
-      <c r="F22" s="37"/>
-      <c r="G22" s="38"/>
+      <c r="D22" s="38"/>
+      <c r="E22" s="38"/>
+      <c r="F22" s="38"/>
+      <c r="G22" s="39"/>
       <c r="H22" s="18"/>
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
@@ -1563,17 +1578,17 @@
       <c r="C24" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="D24" s="13" t="s">
-        <v>52</v>
+      <c r="D24" s="49" t="s">
+        <v>64</v>
       </c>
       <c r="E24" s="21" t="s">
-        <v>25</v>
+        <v>65</v>
       </c>
       <c r="F24" s="21" t="s">
-        <v>24</v>
+        <v>66</v>
       </c>
       <c r="G24" s="21" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="H24" s="22"/>
       <c r="I24" s="4"/>
@@ -1686,16 +1701,16 @@
     <row r="28" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
-      <c r="C28" s="42" t="s">
-        <v>27</v>
+      <c r="C28" s="45" t="s">
+        <v>25</v>
       </c>
-      <c r="D28" s="37"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="37"/>
-      <c r="G28" s="37"/>
-      <c r="H28" s="37"/>
-      <c r="I28" s="37"/>
-      <c r="J28" s="38"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="38"/>
+      <c r="I28" s="38"/>
+      <c r="J28" s="39"/>
       <c r="K28" s="4"/>
       <c r="L28" s="4"/>
       <c r="M28" s="4"/>
@@ -1721,22 +1736,22 @@
         <v>20</v>
       </c>
       <c r="D29" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F29" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="E29" s="8" t="s">
+      <c r="G29" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="F29" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="G29" s="7" t="s">
-        <v>31</v>
-      </c>
       <c r="H29" s="8" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="J29" s="19" t="s">
         <v>14</v>
@@ -1769,22 +1784,22 @@
         <v>11</v>
       </c>
       <c r="E30" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F30" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H30" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="F30" s="25" t="s">
-        <v>36</v>
+      <c r="I30" s="27" t="s">
+        <v>52</v>
       </c>
-      <c r="G30" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="H30" s="26" t="s">
-        <v>38</v>
-      </c>
-      <c r="I30" s="27" t="s">
-        <v>55</v>
-      </c>
-      <c r="J30" s="13" t="s">
-        <v>56</v>
+      <c r="J30" s="49" t="s">
+        <v>65</v>
       </c>
       <c r="K30" s="4"/>
       <c r="L30" s="4"/>
@@ -1894,17 +1909,17 @@
     <row r="34" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
-      <c r="C34" s="44" t="s">
-        <v>32</v>
+      <c r="C34" s="47" t="s">
+        <v>30</v>
       </c>
-      <c r="D34" s="37"/>
-      <c r="E34" s="37"/>
-      <c r="F34" s="38"/>
+      <c r="D34" s="38"/>
+      <c r="E34" s="38"/>
+      <c r="F34" s="39"/>
       <c r="G34" s="4"/>
-      <c r="H34" s="46"/>
-      <c r="I34" s="39"/>
-      <c r="J34" s="39"/>
-      <c r="K34" s="39"/>
+      <c r="H34" s="40"/>
+      <c r="I34" s="41"/>
+      <c r="J34" s="41"/>
+      <c r="K34" s="41"/>
       <c r="L34" s="4"/>
       <c r="M34" s="4"/>
       <c r="N34" s="4"/>
@@ -1926,16 +1941,16 @@
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="28" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D35" s="25" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E35" s="21" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F35" s="29" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G35" s="4"/>
       <c r="H35" s="30"/>
@@ -1966,10 +1981,10 @@
         <v>23</v>
       </c>
       <c r="D36" s="21" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E36" s="21" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F36" s="29" t="s">
         <v>11</v>
@@ -2086,16 +2101,16 @@
     <row r="40" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
-      <c r="C40" s="45" t="s">
-        <v>57</v>
+      <c r="C40" s="37" t="s">
+        <v>53</v>
       </c>
-      <c r="D40" s="37"/>
-      <c r="E40" s="37"/>
-      <c r="F40" s="38"/>
+      <c r="D40" s="38"/>
+      <c r="E40" s="38"/>
+      <c r="F40" s="39"/>
       <c r="G40" s="4"/>
-      <c r="H40" s="46"/>
-      <c r="I40" s="39"/>
-      <c r="J40" s="39"/>
+      <c r="H40" s="40"/>
+      <c r="I40" s="41"/>
+      <c r="J40" s="41"/>
       <c r="K40" s="4"/>
       <c r="L40" s="4"/>
       <c r="M40" s="4"/>
@@ -2118,13 +2133,13 @@
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="12" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D41" s="21" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E41" s="21" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F41" s="19" t="s">
         <v>19</v>
@@ -2158,13 +2173,13 @@
         <v>23</v>
       </c>
       <c r="D42" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E42" s="25" t="s">
         <v>12</v>
       </c>
       <c r="F42" s="25" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="G42" s="4"/>
       <c r="H42" s="3"/>
@@ -2278,15 +2293,15 @@
     <row r="46" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
-      <c r="C46" s="47" t="s">
-        <v>60</v>
+      <c r="C46" s="42" t="s">
+        <v>56</v>
       </c>
-      <c r="D46" s="37"/>
-      <c r="E46" s="37"/>
-      <c r="F46" s="37"/>
-      <c r="G46" s="37"/>
-      <c r="H46" s="37"/>
-      <c r="I46" s="38"/>
+      <c r="D46" s="38"/>
+      <c r="E46" s="38"/>
+      <c r="F46" s="38"/>
+      <c r="G46" s="38"/>
+      <c r="H46" s="38"/>
+      <c r="I46" s="39"/>
       <c r="J46" s="4"/>
       <c r="K46" s="4"/>
       <c r="L46" s="4"/>
@@ -2310,25 +2325,25 @@
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="34" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D47" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="E47" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="F47" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="G47" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="H47" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="E47" s="35" t="s">
+      <c r="I47" s="36" t="s">
         <v>62</v>
-      </c>
-      <c r="F47" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="G47" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="H47" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="I47" s="36" t="s">
-        <v>66</v>
       </c>
       <c r="J47" s="4"/>
       <c r="K47" s="4"/>
@@ -2356,22 +2371,22 @@
         <v>23</v>
       </c>
       <c r="D48" s="21" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E48" s="21" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F48" s="21" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G48" s="21" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H48" s="25" t="s">
         <v>12</v>
       </c>
       <c r="I48" s="21" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="J48" s="4"/>
       <c r="K48" s="4"/>
@@ -2453,10 +2468,10 @@
     <row r="51" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
-      <c r="C51" s="46"/>
-      <c r="D51" s="39"/>
-      <c r="E51" s="39"/>
-      <c r="F51" s="39"/>
+      <c r="C51" s="40"/>
+      <c r="D51" s="41"/>
+      <c r="E51" s="41"/>
+      <c r="F51" s="41"/>
       <c r="G51" s="4"/>
       <c r="H51" s="4"/>
       <c r="I51" s="4"/>
@@ -29857,17 +29872,32 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C16:K16"/>
+    <mergeCell ref="C10:J10"/>
+    <mergeCell ref="C28:J28"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="C34:F34"/>
     <mergeCell ref="C40:F40"/>
     <mergeCell ref="C51:F51"/>
     <mergeCell ref="H34:K34"/>
     <mergeCell ref="H40:J40"/>
     <mergeCell ref="C46:I46"/>
-    <mergeCell ref="C16:K16"/>
-    <mergeCell ref="C10:J10"/>
-    <mergeCell ref="C28:J28"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="C34:F34"/>
   </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0D705C9-95E5-4D66-A67F-2679524C474C}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
scope and feature edit 2
</commit_message>
<xml_diff>
--- a/Documents/Database.xlsx
+++ b/Documents/Database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Group15 Git\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAB19340-05EF-4912-8D55-938A1EA5E6C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFB5121A-6065-4DB8-A3F8-41DE6FB99514}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Database" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="72">
   <si>
     <t>Farmer</t>
   </si>
@@ -238,12 +238,27 @@
   <si>
     <t>Foreign key(Equipment)</t>
   </si>
+  <si>
+    <t>Field</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Null</t>
+  </si>
+  <si>
+    <t>Key</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Default</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -363,6 +378,13 @@
       <b/>
       <sz val="10"/>
       <color theme="4"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -496,7 +518,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -552,21 +574,15 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -579,9 +595,18 @@
     <xf numFmtId="0" fontId="11" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -803,8 +828,8 @@
   </sheetPr>
   <dimension ref="A1:AA995"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I42" sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1096,16 +1121,16 @@
     <row r="10" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
-      <c r="C10" s="44" t="s">
+      <c r="C10" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="38"/>
-      <c r="J10" s="39"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="40"/>
+      <c r="I10" s="40"/>
+      <c r="J10" s="41"/>
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
       <c r="M10" s="4"/>
@@ -1148,7 +1173,7 @@
       <c r="I11" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="J11" s="48" t="s">
+      <c r="J11" s="37" t="s">
         <v>44</v>
       </c>
       <c r="L11" s="4"/>
@@ -1299,17 +1324,17 @@
     <row r="16" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
-      <c r="C16" s="43" t="s">
+      <c r="C16" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="38"/>
-      <c r="E16" s="38"/>
-      <c r="F16" s="38"/>
-      <c r="G16" s="38"/>
-      <c r="H16" s="38"/>
-      <c r="I16" s="38"/>
-      <c r="J16" s="38"/>
-      <c r="K16" s="39"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="40"/>
+      <c r="F16" s="40"/>
+      <c r="G16" s="40"/>
+      <c r="H16" s="40"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="40"/>
+      <c r="K16" s="41"/>
       <c r="L16" s="4"/>
       <c r="M16" s="4"/>
       <c r="N16" s="4"/>
@@ -1506,13 +1531,13 @@
     </row>
     <row r="22" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B22" s="2"/>
-      <c r="C22" s="46" t="s">
+      <c r="C22" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="D22" s="38"/>
-      <c r="E22" s="38"/>
-      <c r="F22" s="38"/>
-      <c r="G22" s="39"/>
+      <c r="D22" s="40"/>
+      <c r="E22" s="40"/>
+      <c r="F22" s="40"/>
+      <c r="G22" s="41"/>
       <c r="H22" s="18"/>
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
@@ -1578,7 +1603,7 @@
       <c r="C24" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="D24" s="49" t="s">
+      <c r="D24" s="38" t="s">
         <v>64</v>
       </c>
       <c r="E24" s="21" t="s">
@@ -1701,16 +1726,16 @@
     <row r="28" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
-      <c r="C28" s="45" t="s">
+      <c r="C28" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="D28" s="38"/>
-      <c r="E28" s="38"/>
-      <c r="F28" s="38"/>
-      <c r="G28" s="38"/>
-      <c r="H28" s="38"/>
-      <c r="I28" s="38"/>
-      <c r="J28" s="39"/>
+      <c r="D28" s="40"/>
+      <c r="E28" s="40"/>
+      <c r="F28" s="40"/>
+      <c r="G28" s="40"/>
+      <c r="H28" s="40"/>
+      <c r="I28" s="40"/>
+      <c r="J28" s="41"/>
       <c r="K28" s="4"/>
       <c r="L28" s="4"/>
       <c r="M28" s="4"/>
@@ -1798,7 +1823,7 @@
       <c r="I30" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="J30" s="49" t="s">
+      <c r="J30" s="38" t="s">
         <v>65</v>
       </c>
       <c r="K30" s="4"/>
@@ -1909,17 +1934,17 @@
     <row r="34" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
-      <c r="C34" s="47" t="s">
+      <c r="C34" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="D34" s="38"/>
-      <c r="E34" s="38"/>
-      <c r="F34" s="39"/>
+      <c r="D34" s="40"/>
+      <c r="E34" s="40"/>
+      <c r="F34" s="41"/>
       <c r="G34" s="4"/>
-      <c r="H34" s="40"/>
-      <c r="I34" s="41"/>
-      <c r="J34" s="41"/>
-      <c r="K34" s="41"/>
+      <c r="H34" s="47"/>
+      <c r="I34" s="48"/>
+      <c r="J34" s="48"/>
+      <c r="K34" s="48"/>
       <c r="L34" s="4"/>
       <c r="M34" s="4"/>
       <c r="N34" s="4"/>
@@ -2101,16 +2126,16 @@
     <row r="40" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
-      <c r="C40" s="37" t="s">
+      <c r="C40" s="46" t="s">
         <v>53</v>
       </c>
-      <c r="D40" s="38"/>
-      <c r="E40" s="38"/>
-      <c r="F40" s="39"/>
+      <c r="D40" s="40"/>
+      <c r="E40" s="40"/>
+      <c r="F40" s="41"/>
       <c r="G40" s="4"/>
-      <c r="H40" s="40"/>
-      <c r="I40" s="41"/>
-      <c r="J40" s="41"/>
+      <c r="H40" s="47"/>
+      <c r="I40" s="48"/>
+      <c r="J40" s="48"/>
       <c r="K40" s="4"/>
       <c r="L40" s="4"/>
       <c r="M40" s="4"/>
@@ -2293,15 +2318,15 @@
     <row r="46" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
-      <c r="C46" s="42" t="s">
+      <c r="C46" s="49" t="s">
         <v>56</v>
       </c>
-      <c r="D46" s="38"/>
-      <c r="E46" s="38"/>
-      <c r="F46" s="38"/>
-      <c r="G46" s="38"/>
-      <c r="H46" s="38"/>
-      <c r="I46" s="39"/>
+      <c r="D46" s="40"/>
+      <c r="E46" s="40"/>
+      <c r="F46" s="40"/>
+      <c r="G46" s="40"/>
+      <c r="H46" s="40"/>
+      <c r="I46" s="41"/>
       <c r="J46" s="4"/>
       <c r="K46" s="4"/>
       <c r="L46" s="4"/>
@@ -2468,10 +2493,10 @@
     <row r="51" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
-      <c r="C51" s="40"/>
-      <c r="D51" s="41"/>
-      <c r="E51" s="41"/>
-      <c r="F51" s="41"/>
+      <c r="C51" s="47"/>
+      <c r="D51" s="48"/>
+      <c r="E51" s="48"/>
+      <c r="F51" s="48"/>
       <c r="G51" s="4"/>
       <c r="H51" s="4"/>
       <c r="I51" s="4"/>
@@ -29872,16 +29897,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C40:F40"/>
+    <mergeCell ref="C51:F51"/>
+    <mergeCell ref="H34:K34"/>
+    <mergeCell ref="H40:J40"/>
+    <mergeCell ref="C46:I46"/>
     <mergeCell ref="C16:K16"/>
     <mergeCell ref="C10:J10"/>
     <mergeCell ref="C28:J28"/>
     <mergeCell ref="C22:G22"/>
     <mergeCell ref="C34:F34"/>
-    <mergeCell ref="C40:F40"/>
-    <mergeCell ref="C51:F51"/>
-    <mergeCell ref="H34:K34"/>
-    <mergeCell ref="H40:J40"/>
-    <mergeCell ref="C46:I46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -29890,14 +29915,45 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0D705C9-95E5-4D66-A67F-2679524C474C}">
-  <dimension ref="A1"/>
+  <dimension ref="E14:I15"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="K16" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="14" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E14" s="50" t="s">
+        <v>0</v>
+      </c>
+      <c r="F14" s="50"/>
+      <c r="G14" s="50"/>
+      <c r="H14" s="50"/>
+      <c r="I14" s="50"/>
+    </row>
+    <row r="15" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
+        <v>67</v>
+      </c>
+      <c r="F15" t="s">
+        <v>68</v>
+      </c>
+      <c r="G15" t="s">
+        <v>69</v>
+      </c>
+      <c r="H15" t="s">
+        <v>70</v>
+      </c>
+      <c r="I15" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E14:I14"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>